<commit_message>
minor code amendments on format of input distribution parameters
</commit_message>
<xml_diff>
--- a/data/analysis_ffd/input/patient_trajectories.xlsx
+++ b/data/analysis_ffd/input/patient_trajectories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucahlgr_ucl_ac_uk/Documents/DesignOfExperiments/ECU_model/R_code/data/an_paper_2_what_if/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucahlgr_ucl_ac_uk/Documents/DesignOfExperiments/ECU_model/DoE_analysis_ECU/data/analysis_ffd/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{0E26D3B1-3102-49B5-9104-E07C3969E927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F75651A6-FA2B-48CD-9D86-A7458E151C4F}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{0E26D3B1-3102-49B5-9104-E07C3969E927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{221C9B99-ECD7-4221-BDFF-9D49CA2228BD}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
   <si>
     <t>Area</t>
   </si>
@@ -52,16 +52,13 @@
     <t>ICU</t>
   </si>
   <si>
-    <t>lognorm,4.8</t>
+    <t>lognorm,0.6,0.06</t>
   </si>
   <si>
-    <t>lognorm,6</t>
+    <t>lognorm,5.4,0.54</t>
   </si>
   <si>
-    <t>lognorm,0.6</t>
-  </si>
-  <si>
-    <t>lognorm,5.4</t>
+    <t>lognorm,4.8,0.48</t>
   </si>
 </sst>
 </file>
@@ -402,7 +399,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -423,7 +420,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -435,6 +432,84 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13791589-F410-41E0-80F1-F73446915465}">
   <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="16384" width="8.83984375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D867DA-85F5-4721-A335-6541D5BBD504}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="16384" width="8.83984375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28326946-83CE-4A10-B07A-B0BDA8CEEA08}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -461,15 +536,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D867DA-85F5-4721-A335-6541D5BBD504}">
-  <dimension ref="A1:B3"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63930FFF-AD04-47BD-A83A-AB72041440FF}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -493,7 +576,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -501,93 +584,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28326946-83CE-4A10-B07A-B0BDA8CEEA08}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="16384" width="8.83984375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63930FFF-AD04-47BD-A83A-AB72041440FF}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="16384" width="8.83984375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -595,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>